<commit_message>
修改：     Book1.xlsx 	新文件：   database/model.mwb
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12315"/>
+    <workbookView windowWidth="28800" windowHeight="12390"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <si>
     <t>user</t>
   </si>
@@ -70,6 +70,9 @@
     <t>varchar(50)</t>
   </si>
   <si>
+    <t>nu,uq</t>
+  </si>
+  <si>
     <t>url</t>
   </si>
   <si>
@@ -95,6 +98,18 @@
   </si>
   <si>
     <t>default  '1.jpeg'</t>
+  </si>
+  <si>
+    <t>money_amout</t>
+  </si>
+  <si>
+    <t>decimal(19,4)</t>
+  </si>
+  <si>
+    <t>nu,default 0</t>
+  </si>
+  <si>
+    <t>frozen_money</t>
   </si>
 </sst>
 </file>
@@ -102,10 +117,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -124,16 +139,113 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -148,61 +260,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -210,51 +270,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -269,13 +284,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -287,31 +380,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,133 +458,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -460,6 +475,56 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -487,43 +552,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -542,165 +575,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1033,10 +1048,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="C3:F16"/>
+  <dimension ref="C3:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
@@ -1141,15 +1156,15 @@
         <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="3:5">
       <c r="C13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -1160,10 +1175,10 @@
     </row>
     <row r="14" spans="3:5">
       <c r="C14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -1171,24 +1186,46 @@
     </row>
     <row r="15" spans="3:5">
       <c r="C15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="3:5">
       <c r="C16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
         <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5">
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5">
+      <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
修改：     Book1.xlsx 	修改：     database/model.mwb 	修改：     database/model.mwb.bak
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12390"/>
+    <workbookView windowWidth="28800" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="73">
   <si>
     <t>user</t>
   </si>
@@ -215,6 +215,24 @@
   </si>
   <si>
     <t>merchant_export_user</t>
+  </si>
+  <si>
+    <t>merchant_rsa_public_keys</t>
+  </si>
+  <si>
+    <t>merchantId</t>
+  </si>
+  <si>
+    <t>pk,fk</t>
+  </si>
+  <si>
+    <t>public_key</t>
+  </si>
+  <si>
+    <t>varchar(500)</t>
+  </si>
+  <si>
+    <t>not null</t>
   </si>
 </sst>
 </file>
@@ -223,15 +241,30 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -239,15 +272,45 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -255,127 +318,82 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -389,187 +407,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -580,6 +598,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -602,6 +629,36 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -612,6 +669,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -630,203 +698,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -839,55 +857,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
-    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
-    <cellStyle name="Total" xfId="25" builtinId="25"/>
-    <cellStyle name="Output" xfId="26" builtinId="21"/>
-    <cellStyle name="Currency" xfId="27" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
-    <cellStyle name="Note" xfId="29" builtinId="10"/>
-    <cellStyle name="Input" xfId="30" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
-    <cellStyle name="Good" xfId="33" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
-    <cellStyle name="Title" xfId="39" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
-    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
-    <cellStyle name="Comma" xfId="44" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
-    <cellStyle name="Percent" xfId="47" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1156,18 +1174,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="C3:F75"/>
+  <dimension ref="C3:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="4.14166666666667" customWidth="true"/>
-    <col min="2" max="2" width="1.11666666666667" customWidth="true"/>
-    <col min="3" max="3" width="23.35" customWidth="true"/>
-    <col min="4" max="4" width="21.575" customWidth="true"/>
+    <col min="1" max="1" width="4.14074074074074" customWidth="true"/>
+    <col min="2" max="2" width="1.11851851851852" customWidth="true"/>
+    <col min="3" max="3" width="23.3481481481481" customWidth="true"/>
+    <col min="4" max="4" width="21.5777777777778" customWidth="true"/>
     <col min="5" max="5" width="34.2666666666667" customWidth="true"/>
   </cols>
   <sheetData>
@@ -1765,6 +1783,33 @@
       </c>
       <c r="E75" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3">
+      <c r="C78" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="79" spans="3:5">
+      <c r="C79" t="s">
+        <v>68</v>
+      </c>
+      <c r="D79" t="s">
+        <v>2</v>
+      </c>
+      <c r="E79" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="80" spans="3:5">
+      <c r="C80" t="s">
+        <v>70</v>
+      </c>
+      <c r="D80" t="s">
+        <v>71</v>
+      </c>
+      <c r="E80" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>